<commit_message>
7.5.10 - bug fixes
</commit_message>
<xml_diff>
--- a/tio-config.xlsx
+++ b/tio-config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creid/Documents/Code/navi/navi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creid/Documents/Code/navi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59A65938-A8EE-F04C-91AB-77091D1E73F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E928CB-EEDC-9F4D-881C-3087CC01FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="-7580" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{BB7F0C85-C231-4C4C-8144-8016471291E9}"/>
+    <workbookView xWindow="-21600" yWindow="-16060" windowWidth="21600" windowHeight="38400" activeTab="4" xr2:uid="{BB7F0C85-C231-4C4C-8144-8016471291E9}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>tag_value</t>
   </si>
@@ -126,97 +126,10 @@
     <t>search_string</t>
   </si>
   <si>
-    <t>docker host</t>
-  </si>
-  <si>
-    <t>plugin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">splunk </t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>splunk</t>
-  </si>
-  <si>
-    <t>applications</t>
-  </si>
-  <si>
-    <t>jira</t>
-  </si>
-  <si>
-    <t>jenkins</t>
-  </si>
-  <si>
-    <t>confluence</t>
-  </si>
-  <si>
-    <t>Tenable Security Center</t>
-  </si>
-  <si>
-    <t>Nessus Scanner</t>
-  </si>
-  <si>
-    <t>Pi-Hole</t>
-  </si>
-  <si>
-    <t>VMWare Host</t>
-  </si>
-  <si>
-    <t>Unitrends</t>
-  </si>
-  <si>
-    <t>Synology NAS</t>
-  </si>
-  <si>
-    <t>PfSense Firewall</t>
-  </si>
-  <si>
-    <t>Device Type</t>
-  </si>
-  <si>
-    <t>DNS Server</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>Wireless Access Point</t>
-  </si>
-  <si>
-    <t>pi-hole</t>
-  </si>
-  <si>
-    <t>unitrends</t>
-  </si>
-  <si>
-    <t>switch</t>
-  </si>
-  <si>
-    <t>Chrome Cast</t>
-  </si>
-  <si>
-    <t>Nintendo</t>
-  </si>
-  <si>
-    <t>nintendo</t>
-  </si>
-  <si>
-    <t>Google TV</t>
-  </si>
-  <si>
-    <t>UAP-AC-PRO</t>
-  </si>
-  <si>
     <t>option</t>
   </si>
   <si>
     <t>option_text</t>
-  </si>
-  <si>
-    <t>Dns Server</t>
   </si>
   <si>
     <t>Linux Systems</t>
@@ -684,20 +597,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>A2</f>
         <v>Aaron@test.ctf</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1732,7 +1645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FFC418-DA49-CD44-A693-47380AC65ADB}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2601,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -2617,8 +2530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6509340-F81B-0141-86FF-ECDB87AE3CCD}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2643,303 +2556,47 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
-        <v>93561</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3">
-        <v>22869</v>
-      </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4">
-        <v>131566</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5">
-        <v>22869</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6">
-        <v>159464</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7">
-        <v>71158</v>
-      </c>
+      <c r="A7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8">
-        <v>10147</v>
-      </c>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>24260</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
+      <c r="A9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>20301</v>
-      </c>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>35291</v>
-      </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12">
-        <v>72341</v>
-      </c>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13">
-        <v>106952</v>
-      </c>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15">
-        <v>54615</v>
-      </c>
-      <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16">
-        <v>10800</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17">
-        <v>10863</v>
-      </c>
-      <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18">
-        <v>10267</v>
-      </c>
-      <c r="E18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
8.3.0 - Added a zipper table to zipper Plugin and highest EPSS value for easy exports
</commit_message>
<xml_diff>
--- a/tio-config.xlsx
+++ b/tio-config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creid/Documents/Code/navi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E928CB-EEDC-9F4D-881C-3087CC01FB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E8C7E2-D94D-184E-90C2-709ECFD74B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-16060" windowWidth="21600" windowHeight="38400" activeTab="4" xr2:uid="{BB7F0C85-C231-4C4C-8144-8016471291E9}"/>
+    <workbookView xWindow="-21600" yWindow="-16060" windowWidth="21600" windowHeight="38400" xr2:uid="{BB7F0C85-C231-4C4C-8144-8016471291E9}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>tag_value</t>
   </si>
@@ -133,15 +133,6 @@
   </si>
   <si>
     <t>Linux Systems</t>
-  </si>
-  <si>
-    <t>Aaron</t>
-  </si>
-  <si>
-    <t>Aaron@test.ctf</t>
-  </si>
-  <si>
-    <t>random1</t>
   </si>
 </sst>
 </file>
@@ -561,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{649CA3B3-D35A-824B-878C-21B4A1F23A24}">
   <dimension ref="A1:H251"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -596,22 +587,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="3" t="str">
-        <f>A2</f>
-        <v>Aaron@test.ctf</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1634,8 +1611,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="hulkhogan@sandbox.io" xr:uid="{754C108A-BAEF-A645-B929-93C4E948CE03}"/>
-    <hyperlink ref="D3:D251" r:id="rId2" display="hulkhogan@sandbox.io" xr:uid="{49CFA02C-C186-1F44-8819-5F08EADF80F9}"/>
+    <hyperlink ref="D3:D251" r:id="rId1" display="hulkhogan@sandbox.io" xr:uid="{49CFA02C-C186-1F44-8819-5F08EADF80F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2530,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6509340-F81B-0141-86FF-ECDB87AE3CCD}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F18"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>